<commit_message>
added first draw of PDU
</commit_message>
<xml_diff>
--- a/Subsystems.xlsx
+++ b/Subsystems.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sun sensors" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="506">
   <si>
     <t xml:space="preserve">Sun sensor</t>
   </si>
@@ -915,6 +915,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://78462f86-a-744dbb28-s-sites.googlegroups.com/a/sinclairinterplanetary.com/www/startrackers/star%20tracker%20RT%202019a.pdf?attachauth=ANoY7cqOQiT_1qMsTvpk-eReb0Q0XdtVi-C_slxqrmkP5SAElh0xXf6vnRgq9olIa6pBrjhe1TCq4DRMdUCwyghKYHQvMhWiBsERskRSkwylgSeTQzKB8e8o-emJVjqa_vVBNZN37YO5NyTD2JJAhsbOUnhQHbP3XssUtNYoeM1hneK8Y0ybcQxH6hXS_DXDUYYkrS8L74QyD2_2UJjOHV22ryS66Ru0OZlInycAPPciva2BrbgichcPTTcuVNCibI33oFAPs7s7&amp;attredirects=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3</t>
   </si>
   <si>
     <t xml:space="preserve">MAI-SS Space Sextant</t>
@@ -1561,7 +1564,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1584,7 +1586,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1592,15 +1593,26 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1655,7 +1667,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1673,6 +1685,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1700,11 +1716,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1712,11 +1740,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1728,23 +1756,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1827,14 +1855,14 @@
   </sheetPr>
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2204,43 +2232,43 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="8" min="5" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="90.4089068825911"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="91.2672064777328"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H2" s="7"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H3" s="7"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="2" t="s">
@@ -2253,625 +2281,637 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="K5" s="7"/>
+        <v>397</v>
+      </c>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="E6" s="10" t="n">
         <v>185</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="10" t="n">
         <v>0.04</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="H6" s="11" t="s">
         <v>399</v>
       </c>
+      <c r="I6" s="11" t="s">
+        <v>400</v>
+      </c>
       <c r="J6" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="K6" s="7"/>
+        <v>401</v>
+      </c>
+      <c r="K6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="F7" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="K7" s="7"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>405</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="B8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>406</v>
-      </c>
-      <c r="F8" s="9" t="n">
+      <c r="E8" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="F8" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="9" t="n">
+      <c r="G8" s="10" t="n">
         <v>0.018</v>
       </c>
-      <c r="H8" s="10" t="n">
+      <c r="H8" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>407</v>
+      <c r="I8" s="11" t="s">
+        <v>408</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="K8" s="7"/>
+        <v>401</v>
+      </c>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="9" t="n">
+      <c r="E9" s="13" t="n">
         <v>226</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="13" t="n">
         <v>20</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="13" t="n">
         <v>0.18</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="I9" s="10" t="s">
+      <c r="H9" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>400</v>
+      <c r="I9" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="E10" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="F10" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="9" t="n">
+      <c r="G10" s="13" t="n">
         <v>0.015</v>
       </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="I10" s="14" t="s">
         <v>415</v>
       </c>
+      <c r="J10" s="12" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="F11" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="G11" s="13" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H11" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>416</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>412</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>417</v>
-      </c>
-      <c r="F11" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="G11" s="9" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="H11" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="C12" s="11" t="s">
         <v>420</v>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="D12" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="F12" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="G12" s="10" t="n">
+      <c r="G12" s="11" t="n">
         <v>0.05</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="I12" s="10" t="s">
+      <c r="H12" s="11" t="s">
         <v>422</v>
       </c>
+      <c r="I12" s="11" t="s">
+        <v>423</v>
+      </c>
       <c r="J12" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="D13" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="10" t="n">
+      <c r="G13" s="11" t="n">
         <v>0.006</v>
       </c>
-      <c r="H13" s="10" t="n">
+      <c r="H13" s="11" t="n">
         <v>0.8</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>426</v>
+      <c r="I13" s="11" t="s">
+        <v>427</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="D14" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="E14" s="11" t="n">
         <v>0.024</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="G14" s="10" t="n">
+      <c r="F14" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="G14" s="11" t="n">
         <v>0.00058</v>
       </c>
-      <c r="H14" s="10" t="n">
+      <c r="H14" s="11" t="n">
         <v>0.625</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>431</v>
+      <c r="I14" s="11" t="s">
+        <v>432</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="E15" s="9" t="n">
+      <c r="C15" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="E15" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="G15" s="9" t="n">
+      <c r="G15" s="10" t="n">
         <v>0.1</v>
       </c>
-      <c r="H15" s="9" t="n">
+      <c r="H15" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>434</v>
+      <c r="I15" s="10" t="s">
+        <v>435</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>437</v>
       </c>
-      <c r="E16" s="10" t="n">
+      <c r="D16" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="E16" s="11" t="n">
         <v>0.137</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="G16" s="10" t="n">
+      <c r="F16" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="G16" s="11" t="n">
         <v>0.02</v>
       </c>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="J16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>440</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="D17" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="E17" s="11" t="n">
         <v>0.06</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="11" t="n">
         <v>0.23</v>
       </c>
-      <c r="G17" s="10" t="n">
+      <c r="G17" s="11" t="n">
         <v>0.0017</v>
       </c>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="11" t="n">
         <v>0.15</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="J17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>444</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="E18" s="11" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F18" s="11" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G18" s="11" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="H18" s="11" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="J18" s="15" t="s">
         <v>445</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="E18" s="10" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="F18" s="10" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="G18" s="10" t="n">
-        <v>0.0036</v>
-      </c>
-      <c r="H18" s="10" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>446</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="E19" s="10" t="n">
+      <c r="C19" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="E19" s="11" t="n">
         <v>0.15</v>
       </c>
-      <c r="F19" s="10" t="n">
+      <c r="F19" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="10" t="n">
+      <c r="G19" s="11" t="n">
         <v>0.01</v>
       </c>
-      <c r="H19" s="10" t="n">
+      <c r="H19" s="11" t="n">
         <v>0.19</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>444</v>
+      <c r="I19" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="16" t="s">
         <v>450</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="17" t="s">
         <v>451</v>
       </c>
-      <c r="E20" s="10" t="n">
+      <c r="D20" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="E20" s="11" t="n">
         <v>0.694</v>
       </c>
-      <c r="F20" s="10" t="n">
+      <c r="F20" s="11" t="n">
         <v>0.635</v>
       </c>
-      <c r="G20" s="10" t="n">
+      <c r="G20" s="11" t="n">
         <v>0.0093</v>
       </c>
-      <c r="H20" s="10" t="n">
+      <c r="H20" s="11" t="n">
         <v>3.17</v>
       </c>
-      <c r="I20" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="J20" s="11" t="s">
+      <c r="I20" s="11" t="s">
         <v>453</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="11" t="s">
         <v>455</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="D21" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="E21" s="11" t="n">
         <v>0.02</v>
       </c>
-      <c r="F21" s="10" t="n">
+      <c r="F21" s="11" t="n">
         <v>0.1</v>
       </c>
-      <c r="G21" s="10" t="n">
+      <c r="G21" s="11" t="n">
         <v>0.002</v>
       </c>
-      <c r="H21" s="10" t="n">
+      <c r="H21" s="11" t="n">
         <v>0.15</v>
       </c>
-      <c r="I21" s="10" t="s">
-        <v>456</v>
+      <c r="I21" s="11" t="s">
+        <v>457</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="K21" s="7" t="s">
         <v>458</v>
       </c>
+      <c r="K21" s="8" t="s">
+        <v>459</v>
+      </c>
       <c r="L21" s="0" t="s">
-        <v>459</v>
-      </c>
-      <c r="M21" s="14" t="s">
         <v>460</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="E22" s="11" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="F22" s="11" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G22" s="11" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H22" s="11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="M22" s="18" t="s">
         <v>461</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="E22" s="10" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="F22" s="10" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G22" s="10" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="H22" s="10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>463</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>464</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="M22" s="14" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="11" t="s">
         <v>467</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10" t="n">
+      <c r="D23" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11" t="n">
         <v>0.5</v>
       </c>
-      <c r="G23" s="10" t="n">
+      <c r="G23" s="11" t="n">
         <v>0.004</v>
       </c>
-      <c r="H23" s="10" t="n">
+      <c r="H23" s="11" t="n">
         <v>0.6</v>
       </c>
-      <c r="I23" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="J23" s="11" t="s">
+      <c r="I23" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="J23" s="15" t="s">
         <v>470</v>
       </c>
-      <c r="M23" s="14" t="s">
-        <v>460</v>
+      <c r="K23" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="E24" s="10" t="n">
+      <c r="D24" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="E24" s="11" t="n">
         <v>0.055</v>
       </c>
-      <c r="F24" s="10" t="n">
+      <c r="F24" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="10" t="n">
+      <c r="G24" s="11" t="n">
         <v>0.015</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10" t="s">
-        <v>473</v>
-      </c>
-      <c r="J24" s="11" t="s">
+      <c r="H24" s="11"/>
+      <c r="I24" s="11" t="s">
         <v>474</v>
       </c>
-      <c r="K24" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="M24" s="15" t="s">
+      <c r="J24" s="15" t="s">
         <v>475</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C25" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="E25" s="10" t="n">
+      <c r="D25" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="E25" s="11" t="n">
         <v>0.26</v>
       </c>
-      <c r="F25" s="10" t="n">
+      <c r="F25" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="G25" s="10" t="n">
+      <c r="G25" s="11" t="n">
         <v>0.04</v>
       </c>
-      <c r="H25" s="10" t="n">
+      <c r="H25" s="11" t="n">
         <v>0.5</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="J25" s="11"/>
+      <c r="I25" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="J25" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2913,20 +2953,20 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3"/>
@@ -2961,165 +3001,165 @@
       <c r="G6" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="18" t="s">
-        <v>479</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="B10" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="D11" s="24" t="s">
+        <v>481</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>481</v>
-      </c>
-      <c r="G11" s="20" t="s">
+      <c r="F11" s="24" t="s">
         <v>482</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>396</v>
+      <c r="G11" s="24" t="s">
+        <v>483</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="21" t="s">
-        <v>483</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="25" t="s">
         <v>484</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="25" t="s">
         <v>485</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="D12" s="25" t="s">
         <v>486</v>
       </c>
-      <c r="F12" s="21" t="n">
+      <c r="E12" s="25" t="s">
+        <v>487</v>
+      </c>
+      <c r="F12" s="25" t="n">
         <v>1160</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="25" t="s">
+        <v>488</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="25" t="s">
+        <v>490</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>491</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>492</v>
+      </c>
+      <c r="E13" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="25" t="n">
+        <v>655</v>
+      </c>
+      <c r="G13" s="25" t="n">
+        <v>280</v>
+      </c>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="25" t="s">
+        <v>493</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>494</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>495</v>
+      </c>
+      <c r="E14" s="25" t="s">
         <v>487</v>
       </c>
-      <c r="H12" s="19" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="21" t="s">
-        <v>489</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>491</v>
-      </c>
-      <c r="E13" s="21" t="n">
+      <c r="F14" s="25" t="n">
+        <v>536</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="25" t="s">
+        <v>496</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>497</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>498</v>
+      </c>
+      <c r="E15" s="25" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>499</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="23" t="s">
+        <v>500</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>501</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>502</v>
+      </c>
+      <c r="E16" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="21" t="n">
-        <v>655</v>
-      </c>
-      <c r="G13" s="21" t="n">
-        <v>280</v>
-      </c>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="21" t="s">
-        <v>492</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>493</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>494</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>486</v>
-      </c>
-      <c r="F14" s="21" t="n">
-        <v>536</v>
-      </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="21" t="s">
-        <v>495</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>496</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>497</v>
-      </c>
-      <c r="E15" s="21" t="n">
-        <v>100</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>498</v>
-      </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="19" t="s">
-        <v>499</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>500</v>
-      </c>
-      <c r="D16" s="19" t="s">
+      <c r="F16" s="23" t="n">
+        <v>110</v>
+      </c>
+      <c r="G16" s="23" t="n">
+        <v>350</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="23" t="s">
+        <v>503</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>501</v>
       </c>
-      <c r="E16" s="19" t="n">
+      <c r="D17" s="23" t="s">
+        <v>504</v>
+      </c>
+      <c r="E17" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="F16" s="19" t="n">
+      <c r="F17" s="23" t="n">
         <v>110</v>
       </c>
-      <c r="G16" s="19" t="n">
-        <v>350</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="19" t="s">
-        <v>502</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>500</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>503</v>
-      </c>
-      <c r="E17" s="19" t="n">
-        <v>2</v>
-      </c>
-      <c r="F17" s="19" t="n">
-        <v>110</v>
-      </c>
-      <c r="G17" s="19" t="n">
+      <c r="G17" s="23" t="n">
         <v>900</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>504</v>
+      <c r="H17" s="23" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3152,7 +3192,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
@@ -3510,8 +3550,8 @@
   </sheetPr>
   <dimension ref="B2:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3790,7 +3830,7 @@
   <dimension ref="B2:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3895,7 +3935,7 @@
   <dimension ref="C2:H8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4045,8 +4085,8 @@
   </sheetPr>
   <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5044,10 +5084,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C3:I17"/>
+  <dimension ref="B3:I17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5055,7 +5095,7 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10526315789474"/>
   </cols>
@@ -5080,7 +5120,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="5"/>
       <c r="C4" s="3" t="s">
         <v>291</v>
       </c>
@@ -5104,11 +5145,14 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>295</v>
+      </c>
       <c r="C5" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0.282</v>
@@ -5119,19 +5163,19 @@
       <c r="G5" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>297</v>
+      <c r="H5" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>0.35</v>
@@ -5143,18 +5187,18 @@
         <v>1.5</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>1.3</v>
@@ -5166,18 +5210,21 @@
         <v>1.5</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>0.04</v>
@@ -5189,18 +5236,21 @@
         <v>0.65</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>306</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0.28</v>
@@ -5212,18 +5262,21 @@
         <v>0.65</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C10" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0.042</v>
@@ -5235,18 +5288,21 @@
         <v>0.65</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>312</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>311</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0.28</v>
@@ -5258,18 +5314,18 @@
         <v>0.7</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.165</v>
@@ -5278,18 +5334,21 @@
         <v>70</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C13" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0.19</v>
@@ -5301,18 +5360,21 @@
         <v>0.5</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C14" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.025</v>
@@ -5324,18 +5386,21 @@
         <v>1</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C15" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0.35</v>
@@ -5347,33 +5412,36 @@
         <v>1</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C16" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E16" s="6" t="n">
+        <v>334</v>
+      </c>
+      <c r="E16" s="7" t="n">
         <v>0.175</v>
       </c>
-      <c r="F16" s="6" t="n">
+      <c r="F16" s="7" t="n">
         <v>60</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5410,12 +5478,12 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5428,7 +5496,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -5446,22 +5514,22 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5469,7 +5537,7 @@
         <v>93</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>2</v>
@@ -5490,7 +5558,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5498,7 +5566,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>5</v>
@@ -5519,7 +5587,7 @@
         <v>18</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5527,7 +5595,7 @@
         <v>93</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>6</v>
@@ -5548,15 +5616,15 @@
         <v>14.5</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0.2</v>
@@ -5577,18 +5645,18 @@
         <v>9</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0.2</v>
@@ -5603,21 +5671,21 @@
         <v>0.196</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0.2</v>
@@ -5632,21 +5700,21 @@
         <v>0.2</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0.3</v>
@@ -5661,18 +5729,18 @@
         <v>0.196</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0.24</v>
@@ -5693,44 +5761,44 @@
         <v>10</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0.19</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>0.007</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0.2</v>
@@ -5751,15 +5819,15 @@
         <v>10.7</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0.5</v>
@@ -5780,15 +5848,15 @@
         <v>11.5</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0.13</v>
@@ -5803,18 +5871,18 @@
         <v>0.046</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1.19</v>
@@ -5829,18 +5897,18 @@
         <v>0.05</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>5</v>
@@ -5855,20 +5923,20 @@
         <v>350</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="D24" s="6" t="n">
+        <v>386</v>
+      </c>
+      <c r="D24" s="7" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="0" t="n">
@@ -5877,22 +5945,22 @@
       <c r="F24" s="3" t="n">
         <v>0.45</v>
       </c>
-      <c r="G24" s="6" t="n">
+      <c r="G24" s="7" t="n">
         <v>0.23</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0.4</v>
@@ -5913,15 +5981,15 @@
         <v>14</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0.1</v>
@@ -5936,13 +6004,13 @@
         <v>0.04</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>3.2</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added architecture block diagram of EPS and PDU
</commit_message>
<xml_diff>
--- a/Subsystems.xlsx
+++ b/Subsystems.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sun sensors" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="512">
   <si>
     <t xml:space="preserve">Sun sensor</t>
   </si>
@@ -362,9 +362,15 @@
     <t xml:space="preserve">GPS receivers</t>
   </si>
   <si>
+    <t xml:space="preserve">Current</t>
+  </si>
+  <si>
     <t xml:space="preserve">Accuracy (m)</t>
   </si>
   <si>
+    <t xml:space="preserve">30mA</t>
+  </si>
+  <si>
     <t xml:space="preserve">SGR-05U</t>
   </si>
   <si>
@@ -395,6 +401,9 @@
     <t xml:space="preserve">https://www.sstl.co.uk/getattachment/Media-Hub/Featured/Navigation/SGR-Axio-Datasheet-2018-V2-Read-Only.pdf?lang=en-GB</t>
   </si>
   <si>
+    <t xml:space="preserve">100mA</t>
+  </si>
+  <si>
     <t xml:space="preserve">OEM615</t>
   </si>
   <si>
@@ -467,6 +476,9 @@
     <t xml:space="preserve">Horizon sensor</t>
   </si>
   <si>
+    <t xml:space="preserve">40mA</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAI-SES Static Earth Sensor</t>
   </si>
   <si>
@@ -482,6 +494,9 @@
     <t xml:space="preserve">https://www.cubesatshop.com/product/mai-ses-ir-earth-sensor/</t>
   </si>
   <si>
+    <t xml:space="preserve">3mA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mini Digital HCI</t>
   </si>
   <si>
@@ -500,10 +515,13 @@
     <t xml:space="preserve">COMMS</t>
   </si>
   <si>
+    <t xml:space="preserve">1A</t>
+  </si>
+  <si>
     <t xml:space="preserve">HISPICO</t>
   </si>
   <si>
-    <t xml:space="preserve">Iqspaceco.</t>
+    <t xml:space="preserve">Iqspaceco</t>
   </si>
   <si>
     <t xml:space="preserve">95x46x15</t>
@@ -1667,7 +1685,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1684,11 +1702,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1862,7 +1884,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2239,36 +2261,36 @@
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="8" min="5" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="91.2672064777328"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="92.0161943319838"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H1" s="8"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H2" s="8"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H3" s="8"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="I4" s="9"/>
+      <c r="C4" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="2" t="s">
@@ -2281,18 +2303,18 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="K5" s="8"/>
+        <v>403</v>
+      </c>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -2301,31 +2323,31 @@
       <c r="B6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="10" t="n">
+      <c r="E6" s="11" t="n">
         <v>185</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="11" t="n">
         <v>0.04</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>400</v>
+      <c r="H6" s="12" t="s">
+        <v>405</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>406</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="K6" s="8"/>
+        <v>407</v>
+      </c>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2334,31 +2356,31 @@
       <c r="B7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="F7" s="10" t="n">
+      <c r="E7" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="F7" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="G7" s="11" t="n">
         <v>0.005</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>405</v>
+      <c r="H7" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>411</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="K7" s="8"/>
+        <v>407</v>
+      </c>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2367,551 +2389,551 @@
       <c r="B8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="H8" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <v>226</v>
+      </c>
+      <c r="F9" s="14" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" s="14" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="F10" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" s="14" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H10" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="10" t="n">
-        <v>0.018</v>
-      </c>
-      <c r="H8" s="11" t="n">
+      <c r="I10" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="F11" s="14" t="n">
+        <v>7</v>
+      </c>
+      <c r="G11" s="14" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H11" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
-        <v>409</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="13" t="n">
-        <v>226</v>
-      </c>
-      <c r="F9" s="13" t="n">
-        <v>20</v>
-      </c>
-      <c r="G9" s="13" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="n">
-        <v>5</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13" t="s">
-        <v>412</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="F10" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" s="13" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="H10" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>415</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="n">
-        <v>6</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="F11" s="13" t="n">
-        <v>7</v>
-      </c>
-      <c r="G11" s="13" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="H11" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>416</v>
+      <c r="I11" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="F12" s="11" t="n">
+      <c r="C12" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="F12" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="G12" s="11" t="n">
+      <c r="G12" s="12" t="n">
         <v>0.05</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>423</v>
+      <c r="H12" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>429</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="C13" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="11" t="n">
+      <c r="G13" s="12" t="n">
         <v>0.006</v>
       </c>
-      <c r="H13" s="11" t="n">
+      <c r="H13" s="12" t="n">
         <v>0.8</v>
       </c>
-      <c r="I13" s="11" t="s">
-        <v>427</v>
+      <c r="I13" s="12" t="s">
+        <v>433</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>429</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="E14" s="11" t="n">
+      <c r="C14" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="E14" s="12" t="n">
         <v>0.024</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>431</v>
-      </c>
-      <c r="G14" s="11" t="n">
+      <c r="F14" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="G14" s="12" t="n">
         <v>0.00058</v>
       </c>
-      <c r="H14" s="11" t="n">
+      <c r="H14" s="12" t="n">
         <v>0.625</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>432</v>
+      <c r="I14" s="12" t="s">
+        <v>438</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="E15" s="10" t="n">
+      <c r="C15" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="E15" s="11" t="n">
         <v>0.5</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="F15" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="G15" s="10" t="n">
+      <c r="G15" s="11" t="n">
         <v>0.1</v>
       </c>
-      <c r="H15" s="10" t="n">
+      <c r="H15" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>435</v>
+      <c r="I15" s="11" t="s">
+        <v>441</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>437</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="E16" s="11" t="n">
+      <c r="C16" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="E16" s="12" t="n">
         <v>0.137</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>439</v>
-      </c>
-      <c r="G16" s="11" t="n">
+      <c r="F16" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="G16" s="12" t="n">
         <v>0.02</v>
       </c>
-      <c r="H16" s="11" t="n">
+      <c r="H16" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="11" t="s">
-        <v>440</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>441</v>
+      <c r="I16" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="E17" s="11" t="n">
+      <c r="C17" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E17" s="12" t="n">
         <v>0.06</v>
       </c>
-      <c r="F17" s="11" t="n">
+      <c r="F17" s="12" t="n">
         <v>0.23</v>
       </c>
-      <c r="G17" s="11" t="n">
+      <c r="G17" s="12" t="n">
         <v>0.0017</v>
       </c>
-      <c r="H17" s="11" t="n">
+      <c r="H17" s="12" t="n">
         <v>0.15</v>
       </c>
-      <c r="I17" s="11" t="s">
-        <v>444</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>445</v>
+      <c r="I17" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="E18" s="11" t="n">
+      <c r="C18" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E18" s="12" t="n">
         <v>0.09</v>
       </c>
-      <c r="F18" s="11" t="n">
+      <c r="F18" s="12" t="n">
         <v>2.3</v>
       </c>
-      <c r="G18" s="11" t="n">
+      <c r="G18" s="12" t="n">
         <v>0.0036</v>
       </c>
-      <c r="H18" s="11" t="n">
+      <c r="H18" s="12" t="n">
         <v>0.19</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>445</v>
+      <c r="I18" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="E19" s="11" t="n">
+      <c r="C19" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E19" s="12" t="n">
         <v>0.15</v>
       </c>
-      <c r="F19" s="11" t="n">
+      <c r="F19" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="11" t="n">
+      <c r="G19" s="12" t="n">
         <v>0.01</v>
       </c>
-      <c r="H19" s="11" t="n">
+      <c r="H19" s="12" t="n">
         <v>0.19</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>445</v>
+      <c r="I19" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>450</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>451</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="E20" s="11" t="n">
+      <c r="B20" s="17" t="s">
+        <v>456</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="E20" s="12" t="n">
         <v>0.694</v>
       </c>
-      <c r="F20" s="11" t="n">
+      <c r="F20" s="12" t="n">
         <v>0.635</v>
       </c>
-      <c r="G20" s="11" t="n">
+      <c r="G20" s="12" t="n">
         <v>0.0093</v>
       </c>
-      <c r="H20" s="11" t="n">
+      <c r="H20" s="12" t="n">
         <v>3.17</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>454</v>
+      <c r="I20" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>455</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="E21" s="11" t="n">
+      <c r="C21" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="E21" s="12" t="n">
         <v>0.02</v>
       </c>
-      <c r="F21" s="11" t="n">
+      <c r="F21" s="12" t="n">
         <v>0.1</v>
       </c>
-      <c r="G21" s="11" t="n">
+      <c r="G21" s="12" t="n">
         <v>0.002</v>
       </c>
-      <c r="H21" s="11" t="n">
+      <c r="H21" s="12" t="n">
         <v>0.15</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>457</v>
+      <c r="I21" s="12" t="s">
+        <v>463</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>459</v>
+        <v>464</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>465</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>460</v>
-      </c>
-      <c r="M21" s="18" t="s">
-        <v>461</v>
+        <v>466</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="E22" s="11" t="n">
+      <c r="C22" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="E22" s="12" t="n">
         <v>0.18</v>
       </c>
-      <c r="F22" s="11" t="n">
+      <c r="F22" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="G22" s="11" t="n">
+      <c r="G22" s="12" t="n">
         <v>0.019</v>
       </c>
-      <c r="H22" s="11" t="n">
+      <c r="H22" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="I22" s="11" t="s">
-        <v>464</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>465</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>466</v>
-      </c>
-      <c r="M22" s="18" t="s">
-        <v>461</v>
+      <c r="I22" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="12" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H23" s="12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>476</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="M23" s="19" t="s">
         <v>467</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>468</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G23" s="11" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="H23" s="11" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>470</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="M23" s="18" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>473</v>
-      </c>
-      <c r="E24" s="11" t="n">
+      <c r="C24" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="E24" s="12" t="n">
         <v>0.055</v>
       </c>
-      <c r="F24" s="11" t="n">
+      <c r="F24" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="11" t="n">
+      <c r="G24" s="12" t="n">
         <v>0.015</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="M24" s="19" t="s">
-        <v>476</v>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>477</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>478</v>
-      </c>
-      <c r="E25" s="11" t="n">
+      <c r="C25" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="E25" s="12" t="n">
         <v>0.26</v>
       </c>
-      <c r="F25" s="11" t="n">
+      <c r="F25" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="G25" s="11" t="n">
+      <c r="G25" s="12" t="n">
         <v>0.04</v>
       </c>
-      <c r="H25" s="11" t="n">
+      <c r="H25" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="I25" s="11" t="s">
-        <v>479</v>
-      </c>
-      <c r="J25" s="15"/>
+      <c r="I25" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="J25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2953,20 +2975,20 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3"/>
@@ -3001,165 +3023,165 @@
       <c r="G6" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="22" t="s">
-        <v>480</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
+      <c r="B10" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>481</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>487</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>482</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>483</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>397</v>
+      <c r="F11" s="25" t="s">
+        <v>488</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>489</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="25" t="s">
-        <v>484</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>485</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>486</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>487</v>
-      </c>
-      <c r="F12" s="25" t="n">
+      <c r="B12" s="26" t="s">
+        <v>490</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>491</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>492</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>493</v>
+      </c>
+      <c r="F12" s="26" t="n">
         <v>1160</v>
       </c>
-      <c r="G12" s="25" t="s">
-        <v>488</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>489</v>
+      <c r="G12" s="26" t="s">
+        <v>494</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="25" t="s">
-        <v>490</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>491</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>492</v>
-      </c>
-      <c r="E13" s="25" t="n">
+      <c r="B13" s="26" t="s">
+        <v>496</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>497</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>498</v>
+      </c>
+      <c r="E13" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="25" t="n">
+      <c r="F13" s="26" t="n">
         <v>655</v>
       </c>
-      <c r="G13" s="25" t="n">
+      <c r="G13" s="26" t="n">
         <v>280</v>
       </c>
-      <c r="H13" s="26"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="26" t="s">
+        <v>499</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>500</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>501</v>
+      </c>
+      <c r="E14" s="26" t="s">
         <v>493</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>494</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>495</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>487</v>
-      </c>
-      <c r="F14" s="25" t="n">
+      <c r="F14" s="26" t="n">
         <v>536</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="23"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="25" t="s">
-        <v>496</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="E15" s="25" t="n">
+      <c r="B15" s="26" t="s">
+        <v>502</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>504</v>
+      </c>
+      <c r="E15" s="26" t="n">
         <v>100</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>499</v>
-      </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="23"/>
+      <c r="F15" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="G15" s="26"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="23" t="s">
-        <v>500</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>501</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>502</v>
-      </c>
-      <c r="E16" s="23" t="n">
+      <c r="B16" s="24" t="s">
+        <v>506</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>507</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>508</v>
+      </c>
+      <c r="E16" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="F16" s="23" t="n">
+      <c r="F16" s="24" t="n">
         <v>110</v>
       </c>
-      <c r="G16" s="23" t="n">
+      <c r="G16" s="24" t="n">
         <v>350</v>
       </c>
-      <c r="H16" s="23" t="s">
-        <v>453</v>
+      <c r="H16" s="24" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="23" t="s">
-        <v>503</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>501</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>504</v>
-      </c>
-      <c r="E17" s="23" t="n">
+      <c r="B17" s="24" t="s">
+        <v>509</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>507</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>510</v>
+      </c>
+      <c r="E17" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="23" t="n">
+      <c r="F17" s="24" t="n">
         <v>110</v>
       </c>
-      <c r="G17" s="23" t="n">
+      <c r="G17" s="24" t="n">
         <v>900</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>505</v>
+      <c r="H17" s="24" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3192,7 +3214,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
@@ -3548,10 +3570,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:H13"/>
+  <dimension ref="A2:S13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3569,6 +3591,9 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>110</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3579,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>59</v>
@@ -3589,11 +3614,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>112</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0.04</v>
@@ -3605,64 +3633,91 @@
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="4" t="n">
         <v>0.45</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="5" t="n">
         <v>1.6</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="H5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="5" t="n">
         <v>0.95</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>123</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>0.021</v>
@@ -3674,18 +3729,21 @@
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>0.024</v>
@@ -3697,102 +3755,106 @@
         <v>0.5</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="0" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="4" t="n">
         <v>0.64</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="4" t="n">
         <v>2.5</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="G9" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="H9" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="4" t="n">
         <v>1.4</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="G10" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="H10" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="4" t="n">
         <v>0.022</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="4" t="n">
         <v>1.6</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="s">
+      <c r="G11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="4" t="n">
         <v>0.138</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="4" t="n">
         <v>1.2</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>143</v>
+      <c r="G12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3827,10 +3889,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:H5"/>
+  <dimension ref="A2:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3840,7 +3902,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3863,54 +3925,60 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>148</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>33</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0.132</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>154</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>50</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0.024</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3932,20 +4000,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C2:H8"/>
+  <dimension ref="B2:H8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3965,16 +4035,19 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>161</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>0.1</v>
@@ -3983,18 +4056,18 @@
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="3" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0.42</v>
@@ -4003,18 +4076,18 @@
         <v>13</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.42</v>
@@ -4023,18 +4096,18 @@
         <v>13</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0.2</v>
@@ -4043,10 +4116,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4085,8 +4158,8 @@
   </sheetPr>
   <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4096,7 +4169,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4117,16 +4190,16 @@
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0.23</v>
@@ -4135,18 +4208,18 @@
         <v>1.26</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0.48</v>
@@ -4155,18 +4228,18 @@
         <v>3.5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1.35</v>
@@ -4175,18 +4248,18 @@
         <v>3.5</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0.15</v>
@@ -4195,18 +4268,18 @@
         <v>1</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0.1</v>
@@ -4215,38 +4288,38 @@
         <v>2.6</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0.12</v>
@@ -4255,18 +4328,18 @@
         <v>0.2</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1.1</v>
@@ -4275,18 +4348,18 @@
         <v>11</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0.7</v>
@@ -4295,18 +4368,18 @@
         <v>1.5</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0.27</v>
@@ -4315,18 +4388,18 @@
         <v>0.5</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0.05</v>
@@ -4335,18 +4408,18 @@
         <v>0.24</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0.33</v>
@@ -4355,18 +4428,18 @@
         <v>8.7</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0.25</v>
@@ -4375,18 +4448,18 @@
         <v>2.5</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>205</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0.25</v>
@@ -4395,18 +4468,18 @@
         <v>2.5</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1.4</v>
@@ -4415,18 +4488,18 @@
         <v>4.2</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1.2</v>
@@ -4435,18 +4508,18 @@
         <v>4.5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1.2</v>
@@ -4455,18 +4528,18 @@
         <v>4.5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>1.2</v>
@@ -4475,18 +4548,18 @@
         <v>4.5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1.2</v>
@@ -4495,10 +4568,10 @@
         <v>4.5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -4533,7 +4606,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4550,39 +4623,39 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="I3" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0.012</v>
@@ -4597,30 +4670,30 @@
         <v>0.235</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="Q4" s="0" t="n">
         <v>482.33</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0.016</v>
@@ -4635,24 +4708,24 @@
         <v>0.165</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.016</v>
@@ -4667,10 +4740,10 @@
         <v>0.25</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="Q6" s="0" t="n">
         <v>633</v>
@@ -4678,16 +4751,16 @@
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>6.25</v>
@@ -4699,10 +4772,10 @@
         <v>0.6</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="Q7" s="0" t="n">
         <v>1.697</v>
@@ -4710,16 +4783,16 @@
     </row>
     <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>0.016</v>
@@ -4734,10 +4807,10 @@
         <v>0.35</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="Q8" s="0" t="n">
         <v>625</v>
@@ -4745,19 +4818,19 @@
     </row>
     <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>15</v>
@@ -4766,24 +4839,24 @@
         <v>0.6</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>28</v>
@@ -4795,27 +4868,27 @@
         <v>0.6</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>15</v>
@@ -4824,21 +4897,21 @@
         <v>1.3</v>
       </c>
       <c r="I11" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>262</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.055</v>
@@ -4853,21 +4926,21 @@
         <v>1.5</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0.052</v>
@@ -4882,21 +4955,21 @@
         <v>1.5</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.055</v>
@@ -4911,21 +4984,21 @@
         <v>1.5</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0.01</v>
@@ -4940,21 +5013,21 @@
         <v>0.05</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0.01</v>
@@ -4969,21 +5042,21 @@
         <v>0.05</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>271</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.01</v>
@@ -4998,24 +5071,24 @@
         <v>0.05</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.015</v>
@@ -5027,24 +5100,24 @@
         <v>0.2</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0.016</v>
@@ -5056,10 +5129,10 @@
         <v>0.3</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -5095,7 +5168,7 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10526315789474"/>
   </cols>
@@ -5108,10 +5181,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>5</v>
@@ -5121,12 +5194,12 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="3" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>0.185</v>
@@ -5138,21 +5211,21 @@
         <v>0.5</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0.282</v>
@@ -5163,19 +5236,19 @@
       <c r="G5" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>298</v>
+      <c r="H5" s="7" t="s">
+        <v>304</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>0.35</v>
@@ -5187,18 +5260,18 @@
         <v>1.5</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>1.3</v>
@@ -5210,10 +5283,10 @@
         <v>1.5</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5221,10 +5294,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>0.04</v>
@@ -5236,10 +5309,10 @@
         <v>0.65</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5247,10 +5320,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0.28</v>
@@ -5262,10 +5335,10 @@
         <v>0.65</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5273,10 +5346,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0.042</v>
@@ -5288,10 +5361,10 @@
         <v>0.65</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5299,10 +5372,10 @@
         <v>5</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0.28</v>
@@ -5314,18 +5387,18 @@
         <v>0.7</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.165</v>
@@ -5334,10 +5407,10 @@
         <v>70</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5345,10 +5418,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0.19</v>
@@ -5360,10 +5433,10 @@
         <v>0.5</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5371,10 +5444,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.025</v>
@@ -5386,10 +5459,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5397,10 +5470,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0.35</v>
@@ -5412,10 +5485,10 @@
         <v>1</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5423,25 +5496,25 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E16" s="7" t="n">
+        <v>340</v>
+      </c>
+      <c r="E16" s="8" t="n">
         <v>0.175</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="8" t="n">
         <v>60</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5478,12 +5551,12 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5496,7 +5569,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -5507,29 +5580,29 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>343</v>
+      <c r="D9" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5537,7 +5610,7 @@
         <v>93</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>2</v>
@@ -5558,7 +5631,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5566,7 +5639,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>5</v>
@@ -5587,7 +5660,7 @@
         <v>18</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5595,7 +5668,7 @@
         <v>93</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>6</v>
@@ -5616,15 +5689,15 @@
         <v>14.5</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0.2</v>
@@ -5645,18 +5718,18 @@
         <v>9</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0.2</v>
@@ -5671,21 +5744,21 @@
         <v>0.196</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0.2</v>
@@ -5700,21 +5773,21 @@
         <v>0.2</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0.3</v>
@@ -5729,18 +5802,18 @@
         <v>0.196</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0.24</v>
@@ -5761,44 +5834,44 @@
         <v>10</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0.19</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>0.007</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0.2</v>
@@ -5819,15 +5892,15 @@
         <v>10.7</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0.5</v>
@@ -5848,15 +5921,15 @@
         <v>11.5</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0.13</v>
@@ -5871,18 +5944,18 @@
         <v>0.046</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1.19</v>
@@ -5897,18 +5970,18 @@
         <v>0.05</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>5</v>
@@ -5923,20 +5996,20 @@
         <v>350</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D24" s="7" t="n">
+        <v>392</v>
+      </c>
+      <c r="D24" s="8" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="0" t="n">
@@ -5945,22 +6018,22 @@
       <c r="F24" s="3" t="n">
         <v>0.45</v>
       </c>
-      <c r="G24" s="7" t="n">
+      <c r="G24" s="8" t="n">
         <v>0.23</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0.4</v>
@@ -5981,15 +6054,15 @@
         <v>14</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0.1</v>
@@ -6004,13 +6077,13 @@
         <v>0.04</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>3.2</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>